<commit_message>
Started work on data loading logic
</commit_message>
<xml_diff>
--- a/LOEViz_base/project_state.xlsx
+++ b/LOEViz_base/project_state.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MattM\Documents\LOEViz\LOEViz_base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94FA91B-3034-4170-86D4-56789F70C445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4842E1E2-518F-40DD-9345-97E98A1EBF2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{27414D50-8B9E-4081-AF1D-9D832E49670B}"/>
   </bookViews>
@@ -474,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6DF7A01-9305-43F1-BD11-14BB09DB169C}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -653,13 +653,18 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="J23">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Integrated Excel loading into existing logic
Also, bugfixes!
</commit_message>
<xml_diff>
--- a/LOEViz_base/project_state.xlsx
+++ b/LOEViz_base/project_state.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MattM\Documents\LOEViz\LOEViz_base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65391DB6-7A63-4FD0-96EF-9CC4F3070E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7989F1DB-83C5-459E-9B9F-0D8A141D1B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{27414D50-8B9E-4081-AF1D-9D832E49670B}"/>
   </bookViews>
@@ -477,7 +477,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,7 +582,7 @@
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added arrows to show dependencies
</commit_message>
<xml_diff>
--- a/LOEViz_base/project_state.xlsx
+++ b/LOEViz_base/project_state.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MattM\Documents\LOEViz\LOEViz_base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443636E9-8B0B-4ABE-95E8-CD1158594B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6345C441-8052-45EC-8CDB-E97FAFD073AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{27414D50-8B9E-4081-AF1D-9D832E49670B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -72,6 +72,9 @@
     <t>O2.1</t>
   </si>
   <si>
+    <t>IO1.1.1</t>
+  </si>
+  <si>
     <t>O1.1,O1.2</t>
   </si>
   <si>
@@ -81,9 +84,6 @@
     <t>On Track</t>
   </si>
   <si>
-    <t>Complete</t>
-  </si>
-  <si>
     <t>Project visualization tool</t>
   </si>
   <si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Unload boxes</t>
+  </si>
+  <si>
+    <t>Create fake data</t>
   </si>
 </sst>
 </file>
@@ -477,7 +480,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,7 +528,7 @@
         <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -542,7 +545,7 @@
         <v>45078</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
         <v>22</v>
@@ -562,7 +565,10 @@
         <v>45061</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -599,7 +605,7 @@
         <v>45058</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -616,14 +622,28 @@
         <v>45071</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C8" s="3"/>
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="3">
+        <v>45056</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45059</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C9" s="3"/>

</xml_diff>

<commit_message>
Added automatic status updating
</commit_message>
<xml_diff>
--- a/LOEViz_base/project_state.xlsx
+++ b/LOEViz_base/project_state.xlsx
@@ -2,37 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MattM\Documents\LOEViz\LOEViz_base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6345C441-8052-45EC-8CDB-E97FAFD073AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37757D0-2BF1-4C94-AA30-8A1AD0583E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{27414D50-8B9E-4081-AF1D-9D832E49670B}"/>
+    <workbookView xWindow="5760" yWindow="72" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOEs, IOs, and Objectives" sheetId="1" r:id="rId1"/>
-    <sheet name="Instructions" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -60,52 +43,52 @@
     <t>LOE1</t>
   </si>
   <si>
+    <t>Project visualization tool</t>
+  </si>
+  <si>
+    <t>At Risk</t>
+  </si>
+  <si>
+    <t>O1.1,O1.2</t>
+  </si>
+  <si>
     <t>LOE2</t>
   </si>
   <si>
+    <t>Moving in</t>
+  </si>
+  <si>
+    <t>On Track</t>
+  </si>
+  <si>
+    <t>O2.1,O2.2</t>
+  </si>
+  <si>
     <t>O1.1</t>
   </si>
   <si>
+    <t>Write input and validation logic</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>IO1.1.1</t>
+  </si>
+  <si>
     <t>O1.2</t>
   </si>
   <si>
+    <t>Create visual logic</t>
+  </si>
+  <si>
     <t>O2.1</t>
   </si>
   <si>
-    <t>IO1.1.1</t>
-  </si>
-  <si>
-    <t>O1.1,O1.2</t>
-  </si>
-  <si>
-    <t>Overdue</t>
-  </si>
-  <si>
-    <t>On Track</t>
-  </si>
-  <si>
-    <t>Project visualization tool</t>
-  </si>
-  <si>
-    <t>Moving in</t>
-  </si>
-  <si>
-    <t>At Risk</t>
-  </si>
-  <si>
     <t>Clean out room</t>
   </si>
   <si>
-    <t>Write input and validation logic</t>
-  </si>
-  <si>
-    <t>Create visual logic</t>
-  </si>
-  <si>
     <t>O2.2</t>
-  </si>
-  <si>
-    <t>O2.1,O2.2</t>
   </si>
   <si>
     <t>Unload boxes</t>
@@ -119,7 +102,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -132,10 +115,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -146,7 +126,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -154,21 +134,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -191,44 +187,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -255,32 +251,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -307,24 +285,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -336,159 +296,182 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6DF7A01-9305-43F1-BD11-14BB09DB169C}">
-  <dimension ref="A1:F18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="35.33203125" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
-    <col min="6" max="6" width="26.5546875" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -516,187 +499,136 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="3">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2">
         <v>45056</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>45066</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="3">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2">
         <v>45054</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>45078</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="3">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2">
         <v>45056</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>45061</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="3">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2">
         <v>45060</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>45065</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="3">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2">
         <v>45055</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>45058</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>45060</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>45071</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>45056</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>45059</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20417367-652F-4D11-9FD9-F2F5ECC4D810}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>